<commit_message>
- apply home dialog texts from excel
</commit_message>
<xml_diff>
--- a/resource/texts/SDTexts.xlsx
+++ b/resource/texts/SDTexts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Apps_Win\SchoolDatabase\trunk\resource\texts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9FB659-E913-42BE-A7D7-DB5E95C357EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E965A-1BA2-4BA3-A8E2-7275831D22EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>STR_SCHOOL_YEAR</t>
   </si>
@@ -50,6 +49,48 @@
   </si>
   <si>
     <t>Contoh</t>
+  </si>
+  <si>
+    <t>STR_HOME_TITLE</t>
+  </si>
+  <si>
+    <t>Welcome to School Database</t>
+  </si>
+  <si>
+    <t>Main Menu</t>
+  </si>
+  <si>
+    <t>STR_MAIN_MENU</t>
+  </si>
+  <si>
+    <t>STR_DB_STUDENT</t>
+  </si>
+  <si>
+    <t>Student DB</t>
+  </si>
+  <si>
+    <t>STR_DB_CLASS</t>
+  </si>
+  <si>
+    <t>Class DB</t>
+  </si>
+  <si>
+    <t>STR_DB_EMPLOYEE</t>
+  </si>
+  <si>
+    <t>Employee DB</t>
+  </si>
+  <si>
+    <t>STR_DB_COURSE</t>
+  </si>
+  <si>
+    <t>Course DB</t>
+  </si>
+  <si>
+    <t>STR_DB_INVENTORY</t>
+  </si>
+  <si>
+    <t>Inventory DB</t>
   </si>
 </sst>
 </file>
@@ -370,16 +411,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -415,6 +457,62 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ add Student DB & it's register dialog
</commit_message>
<xml_diff>
--- a/resource/texts/SDTexts.xlsx
+++ b/resource/texts/SDTexts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Apps_Win\SchoolDatabase\trunk\resource\texts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E965A-1BA2-4BA3-A8E2-7275831D22EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B90D35-ADA3-471E-A4AE-BA7023D947D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>STR_SCHOOL_YEAR</t>
   </si>
@@ -91,6 +91,36 @@
   </si>
   <si>
     <t>Inventory DB</t>
+  </si>
+  <si>
+    <t>STR_NEW</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>STR_STUDENT_NAME_LIST</t>
+  </si>
+  <si>
+    <t>Student List</t>
+  </si>
+  <si>
+    <t>STR_NAME</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>STR_BIRTH_PLACE</t>
+  </si>
+  <si>
+    <t>Place of birth</t>
+  </si>
+  <si>
+    <t>STR_BIRTH_DATE</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
   </si>
 </sst>
 </file>
@@ -411,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +543,46 @@
         <v>21</v>
       </c>
     </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>